<commit_message>
(feat):restrict excel out put form
</commit_message>
<xml_diff>
--- a/1213_timetable.xlsx
+++ b/1213_timetable.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,27 +26,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Tahoma"/>
       <b val="1"/>
       <color rgb="000000FF"/>
+      <sz val="11"/>
     </font>
     <font>
+      <name val="Tahoma"/>
+      <b val="1"/>
+      <color rgb="00000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <b val="1"/>
+      <color rgb="00FF0000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
       <b val="1"/>
       <color rgb="00000000"/>
     </font>
     <font>
-      <b val="1"/>
-      <color rgb="00FF0000"/>
+      <name val="Tahoma"/>
+      <sz val="11"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C0C0C0"/>
+        <bgColor rgb="00C0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E0FFFF"/>
+        <bgColor rgb="00E0FFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -54,11 +81,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -69,6 +102,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -143,6 +183,36 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1533525" cy="723900"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -447,6 +517,7 @@
     <col width="87.67" customWidth="1" min="3" max="3"/>
     <col width="25.67" customWidth="1" min="4" max="4"/>
     <col width="14.33" customWidth="1" min="5" max="5"/>
+    <col width="14.33" customWidth="1" min="6" max="6"/>
     <col width="24.5" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -507,255 +578,256 @@
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="9" ht="30" customHeight="1">
+      <c r="A9" s="4" t="inlineStr">
         <is>
           <t>Day</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="4" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="4" t="inlineStr">
         <is>
           <t>Unit</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Classroom Level/ Room/ Venue</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t>Classroom
+Level/ Room/ Venue</t>
+        </is>
+      </c>
+      <c r="E9" s="4" t="inlineStr">
         <is>
           <t>Lecturer</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" s="4" t="inlineStr">
         <is>
           <t>Tutor</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G9" s="4" t="inlineStr">
         <is>
           <t>Delivery Mode</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>monday</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B10" s="6" t="inlineStr">
         <is>
           <t>8:00 to 9:00(L + T)</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="6" t="inlineStr">
         <is>
           <t>MITS5003-(1h Lecture 1)</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" s="6" t="n">
         <v>1234</v>
       </c>
-      <c r="E10" t="n">
-        <v/>
-      </c>
-      <c r="F10" t="n">
-        <v/>
-      </c>
-      <c r="G10" t="inlineStr">
+      <c r="E10" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v/>
+      </c>
+      <c r="G10" s="6" t="inlineStr">
         <is>
           <t>oncampus</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>thursday</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B11" s="6" t="inlineStr">
         <is>
           <t>15:00 to 16:30(L + T)</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="6" t="inlineStr">
         <is>
           <t>MITS6002-(1h30min Lecture 1)</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="D11" s="6" t="n">
         <v>1234</v>
       </c>
-      <c r="E11" t="n">
-        <v/>
-      </c>
-      <c r="F11" t="n">
-        <v/>
-      </c>
-      <c r="G11" t="inlineStr">
+      <c r="E11" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F11" s="6" t="n">
+        <v/>
+      </c>
+      <c r="G11" s="6" t="inlineStr">
         <is>
           <t>oncampus</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>friday</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="inlineStr">
         <is>
           <t>8:00 to 9:00(L + T)</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="6" t="inlineStr">
         <is>
           <t>MITS5003-(1h Tutorial 1)</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" s="6" t="n">
         <v>65432</v>
       </c>
-      <c r="E12" t="n">
-        <v/>
-      </c>
-      <c r="F12" t="n">
-        <v/>
-      </c>
-      <c r="G12" t="inlineStr">
+      <c r="E12" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F12" s="6" t="n">
+        <v/>
+      </c>
+      <c r="G12" s="6" t="inlineStr">
         <is>
           <t>oncampus</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>friday</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="inlineStr">
         <is>
           <t>15:00 to 16:30(L + T)</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="6" t="inlineStr">
         <is>
           <t>MITS6002-(1h30min Lecture 2)</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" s="6" t="n">
         <v>1234</v>
       </c>
-      <c r="E13" t="n">
-        <v/>
-      </c>
-      <c r="F13" t="n">
-        <v/>
-      </c>
-      <c r="G13" t="inlineStr">
+      <c r="E13" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F13" s="6" t="n">
+        <v/>
+      </c>
+      <c r="G13" s="6" t="inlineStr">
         <is>
           <t>oncampus</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>saturday</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="inlineStr">
         <is>
           <t>7:00 to 8:00(L + T)</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="6" t="inlineStr">
         <is>
           <t>MITS5509-(1h Lecture 1)</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" s="6" t="n">
         <v>12345</v>
       </c>
-      <c r="E14" t="n">
-        <v/>
-      </c>
-      <c r="F14" t="n">
-        <v/>
-      </c>
-      <c r="G14" t="inlineStr">
+      <c r="E14" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F14" s="6" t="n">
+        <v/>
+      </c>
+      <c r="G14" s="6" t="inlineStr">
         <is>
           <t>oncampus</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>saturday</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="B15" s="6" t="inlineStr">
         <is>
           <t>12:00 to 13:00(L + T)</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="6" t="inlineStr">
         <is>
           <t>MITS6005-(1h Lecture 1)</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" s="6" t="n">
         <v>1234</v>
       </c>
-      <c r="E15" t="n">
-        <v/>
-      </c>
-      <c r="F15" t="n">
-        <v/>
-      </c>
-      <c r="G15" t="inlineStr">
+      <c r="E15" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F15" s="6" t="n">
+        <v/>
+      </c>
+      <c r="G15" s="6" t="inlineStr">
         <is>
           <t>oncampus</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>sunday</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="B16" s="6" t="inlineStr">
         <is>
           <t>7:00 to 8:00(L + T)</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="6" t="inlineStr">
         <is>
           <t>MITS5509-(1h Lecture 2)</t>
         </is>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" s="6" t="n">
         <v>1234</v>
       </c>
-      <c r="E16" t="n">
-        <v/>
-      </c>
-      <c r="F16" t="n">
-        <v/>
-      </c>
-      <c r="G16" t="inlineStr">
+      <c r="E16" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F16" s="6" t="n">
+        <v/>
+      </c>
+      <c r="G16" s="6" t="inlineStr">
         <is>
           <t>oncampus</t>
         </is>
@@ -772,5 +844,6 @@
     <mergeCell ref="A7:G7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>